<commit_message>
Implemented random_swap.py and random_crop.py
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yimenggu/Desktop/twitter-comms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61A4522-19F5-164C-A62F-871CAF0D8318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A553DAD3-A5EB-3844-9446-2342DF2D263D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30900" yWindow="1460" windowWidth="28040" windowHeight="16200" activeTab="1" xr2:uid="{83E1EE90-11A9-2944-8CCC-8774B4B18D7B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="44">
   <si>
     <t>No.</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>ConDA(BLIP-2)  using z as the input to the classifier instead of h</t>
+  </si>
+  <si>
+    <t>ConDA(BLIP-2) w/ test_time_adaptation()  before validate() w/o triplet loss, using z as the input to the classifier instead of h</t>
   </si>
 </sst>
 </file>
@@ -302,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -359,6 +362,21 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -369,12 +387,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -394,12 +406,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -882,10 +888,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B38549D-5ACE-AD42-90AC-3551968574DA}">
-  <dimension ref="B3:M32"/>
+  <dimension ref="B3:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8:I11"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33:I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -929,10 +935,10 @@
       <c r="M3" s="13"/>
     </row>
     <row r="4" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="34" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="15" t="s">
@@ -950,15 +956,15 @@
       <c r="H4" s="8">
         <v>0.71699999999999997</v>
       </c>
-      <c r="I4" s="35"/>
+      <c r="I4" s="23"/>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
     </row>
     <row r="5" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B5" s="29"/>
-      <c r="C5" s="32"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="17" t="s">
         <v>30</v>
       </c>
@@ -974,15 +980,15 @@
       <c r="H5" s="8">
         <v>0.80800000000000005</v>
       </c>
-      <c r="I5" s="35"/>
+      <c r="I5" s="23"/>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
     </row>
     <row r="6" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B6" s="29"/>
-      <c r="C6" s="32"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="35"/>
       <c r="D6" s="15" t="s">
         <v>31</v>
       </c>
@@ -998,15 +1004,15 @@
       <c r="H6" s="8">
         <v>0.81100000000000005</v>
       </c>
-      <c r="I6" s="35"/>
+      <c r="I6" s="23"/>
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
     </row>
     <row r="7" spans="2:13" ht="21" x14ac:dyDescent="0.2">
-      <c r="B7" s="30"/>
-      <c r="C7" s="33"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="36"/>
       <c r="D7" s="15" t="s">
         <v>23</v>
       </c>
@@ -1022,14 +1028,14 @@
       <c r="H7" s="8">
         <v>0.81100000000000005</v>
       </c>
-      <c r="I7" s="35"/>
+      <c r="I7" s="23"/>
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
       <c r="M7" s="13"/>
     </row>
     <row r="8" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="30" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="26" t="s">
@@ -1050,14 +1056,14 @@
       <c r="H8" s="8">
         <v>0.63700000000000001</v>
       </c>
-      <c r="I8" s="35"/>
+      <c r="I8" s="23"/>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
     </row>
     <row r="9" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B9" s="27"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="26"/>
       <c r="D9" s="17" t="s">
         <v>30</v>
@@ -1074,14 +1080,14 @@
       <c r="H9" s="8">
         <v>0.69299999999999995</v>
       </c>
-      <c r="I9" s="35"/>
+      <c r="I9" s="23"/>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
     </row>
     <row r="10" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B10" s="27"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="26"/>
       <c r="D10" s="15" t="s">
         <v>31</v>
@@ -1098,14 +1104,14 @@
       <c r="H10" s="8">
         <v>0.69799999999999995</v>
       </c>
-      <c r="I10" s="35"/>
+      <c r="I10" s="23"/>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
     </row>
     <row r="11" spans="2:13" ht="20" x14ac:dyDescent="0.2">
-      <c r="B11" s="27"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="26"/>
       <c r="D11" s="19" t="s">
         <v>23</v>
@@ -1122,14 +1128,14 @@
       <c r="H11" s="8">
         <v>0.69699999999999995</v>
       </c>
-      <c r="I11" s="35"/>
+      <c r="I11" s="23"/>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
     </row>
     <row r="12" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="30" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="26" t="s">
@@ -1150,14 +1156,14 @@
       <c r="H12" s="8">
         <v>0.72099999999999997</v>
       </c>
-      <c r="I12" s="35"/>
+      <c r="I12" s="23"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
     </row>
     <row r="13" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B13" s="27"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="26"/>
       <c r="D13" s="17" t="s">
         <v>30</v>
@@ -1174,14 +1180,14 @@
       <c r="H13" s="8">
         <v>0.76800000000000002</v>
       </c>
-      <c r="I13" s="35"/>
+      <c r="I13" s="23"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
     </row>
     <row r="14" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B14" s="27"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="26"/>
       <c r="D14" s="15" t="s">
         <v>31</v>
@@ -1198,14 +1204,14 @@
       <c r="H14" s="8">
         <v>0.77</v>
       </c>
-      <c r="I14" s="35"/>
+      <c r="I14" s="23"/>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
     </row>
     <row r="15" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="30" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="26" t="s">
@@ -1214,7 +1220,7 @@
       <c r="D15" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="27">
         <v>1000</v>
       </c>
       <c r="F15" s="21" t="s">
@@ -1226,19 +1232,19 @@
       <c r="H15" s="8">
         <v>0.78400000000000003</v>
       </c>
-      <c r="I15" s="35"/>
+      <c r="I15" s="23"/>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
     </row>
     <row r="16" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B16" s="27"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="26"/>
       <c r="D16" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="23"/>
+      <c r="E16" s="28"/>
       <c r="F16" s="21" t="s">
         <v>25</v>
       </c>
@@ -1248,19 +1254,19 @@
       <c r="H16" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="35"/>
+      <c r="I16" s="23"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
     </row>
     <row r="17" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B17" s="27"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="26"/>
       <c r="D17" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="24"/>
+      <c r="E17" s="29"/>
       <c r="F17" s="8">
         <v>0.80300000000000005</v>
       </c>
@@ -1270,14 +1276,14 @@
       <c r="H17" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="35"/>
+      <c r="I17" s="23"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
     </row>
     <row r="18" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="30" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="26" t="s">
@@ -1286,7 +1292,7 @@
       <c r="D18" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="27">
         <v>1001</v>
       </c>
       <c r="F18" s="21" t="s">
@@ -1298,19 +1304,19 @@
       <c r="H18" s="8">
         <v>0.78500000000000003</v>
       </c>
-      <c r="I18" s="35"/>
+      <c r="I18" s="23"/>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
     </row>
     <row r="19" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B19" s="27"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="26"/>
       <c r="D19" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="23"/>
+      <c r="E19" s="28"/>
       <c r="F19" s="21" t="s">
         <v>25</v>
       </c>
@@ -1320,19 +1326,19 @@
       <c r="H19" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="35"/>
+      <c r="I19" s="23"/>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
     </row>
     <row r="20" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B20" s="27"/>
+      <c r="B20" s="30"/>
       <c r="C20" s="26"/>
       <c r="D20" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="24"/>
+      <c r="E20" s="29"/>
       <c r="F20" s="8">
         <v>0.80500000000000005</v>
       </c>
@@ -1342,7 +1348,7 @@
       <c r="H20" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="35"/>
+      <c r="I20" s="23"/>
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
@@ -1358,7 +1364,7 @@
       <c r="D21" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="22">
+      <c r="E21" s="27">
         <v>1001</v>
       </c>
       <c r="F21" s="21" t="s">
@@ -1370,7 +1376,7 @@
       <c r="H21" s="8">
         <v>0.79300000000000004</v>
       </c>
-      <c r="I21" s="34" t="s">
+      <c r="I21" s="24" t="s">
         <v>40</v>
       </c>
       <c r="J21" s="13"/>
@@ -1384,7 +1390,7 @@
       <c r="D22" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="23"/>
+      <c r="E22" s="28"/>
       <c r="F22" s="21" t="s">
         <v>25</v>
       </c>
@@ -1394,7 +1400,7 @@
       <c r="H22" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I22" s="34"/>
+      <c r="I22" s="24"/>
       <c r="J22" s="13"/>
       <c r="K22" s="13"/>
       <c r="L22" s="13"/>
@@ -1406,7 +1412,7 @@
       <c r="D23" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="24"/>
+      <c r="E23" s="29"/>
       <c r="F23" s="8">
         <v>0.80200000000000005</v>
       </c>
@@ -1416,7 +1422,7 @@
       <c r="H23" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I23" s="34"/>
+      <c r="I23" s="24"/>
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
       <c r="L23" s="13"/>
@@ -1432,7 +1438,7 @@
       <c r="D24" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="22">
+      <c r="E24" s="27">
         <v>1001</v>
       </c>
       <c r="F24" s="21" t="s">
@@ -1444,7 +1450,7 @@
       <c r="H24" s="8">
         <v>0.78400000000000003</v>
       </c>
-      <c r="I24" s="34"/>
+      <c r="I24" s="24"/>
       <c r="J24" s="13"/>
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
@@ -1456,7 +1462,7 @@
       <c r="D25" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="23"/>
+      <c r="E25" s="28"/>
       <c r="F25" s="21" t="s">
         <v>25</v>
       </c>
@@ -1466,7 +1472,7 @@
       <c r="H25" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I25" s="34"/>
+      <c r="I25" s="24"/>
       <c r="J25" s="13"/>
       <c r="K25" s="13"/>
       <c r="L25" s="13"/>
@@ -1478,7 +1484,7 @@
       <c r="D26" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="24"/>
+      <c r="E26" s="29"/>
       <c r="F26" s="8">
         <v>0.80100000000000005</v>
       </c>
@@ -1488,7 +1494,7 @@
       <c r="H26" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I26" s="34"/>
+      <c r="I26" s="24"/>
       <c r="J26" s="13"/>
       <c r="K26" s="13"/>
       <c r="L26" s="13"/>
@@ -1504,7 +1510,7 @@
       <c r="D27" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="22">
+      <c r="E27" s="27">
         <v>1001</v>
       </c>
       <c r="F27" s="21" t="s">
@@ -1516,7 +1522,7 @@
       <c r="H27" s="8">
         <v>0.79700000000000004</v>
       </c>
-      <c r="I27" s="34" t="s">
+      <c r="I27" s="24" t="s">
         <v>40</v>
       </c>
       <c r="J27" s="13"/>
@@ -1530,7 +1536,7 @@
       <c r="D28" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="23"/>
+      <c r="E28" s="28"/>
       <c r="F28" s="21" t="s">
         <v>25</v>
       </c>
@@ -1540,7 +1546,7 @@
       <c r="H28" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I28" s="34"/>
+      <c r="I28" s="24"/>
       <c r="J28" s="13"/>
       <c r="K28" s="13"/>
       <c r="L28" s="13"/>
@@ -1552,7 +1558,7 @@
       <c r="D29" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="24"/>
+      <c r="E29" s="29"/>
       <c r="F29" s="8">
         <v>0.80300000000000005</v>
       </c>
@@ -1562,15 +1568,15 @@
       <c r="H29" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="34"/>
+      <c r="I29" s="24"/>
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
       <c r="L29" s="13"/>
       <c r="M29" s="13"/>
     </row>
     <row r="30" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B30" s="27" t="s">
-        <v>22</v>
+      <c r="B30" s="25" t="s">
+        <v>43</v>
       </c>
       <c r="C30" s="26" t="s">
         <v>37</v>
@@ -1578,8 +1584,8 @@
       <c r="D30" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E30" s="18" t="s">
-        <v>25</v>
+      <c r="E30" s="27">
+        <v>1001</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>25</v>
@@ -1588,83 +1594,132 @@
         <v>25</v>
       </c>
       <c r="H30" s="8">
-        <v>0.75600000000000001</v>
-      </c>
-      <c r="I30" s="35"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="I30" s="22"/>
       <c r="J30" s="13"/>
       <c r="K30" s="13"/>
       <c r="L30" s="13"/>
       <c r="M30" s="13"/>
     </row>
     <row r="31" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B31" s="27"/>
+      <c r="B31" s="25"/>
       <c r="C31" s="26"/>
       <c r="D31" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="18" t="s">
-        <v>25</v>
-      </c>
+      <c r="E31" s="28"/>
       <c r="F31" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="G31" s="8" t="s">
-        <v>38</v>
+      <c r="G31" s="8">
+        <v>0.80100000000000005</v>
       </c>
       <c r="H31" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I31" s="35"/>
+      <c r="I31" s="22"/>
       <c r="J31" s="13"/>
       <c r="K31" s="13"/>
       <c r="L31" s="13"/>
       <c r="M31" s="13"/>
     </row>
     <row r="32" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B32" s="27"/>
+      <c r="B32" s="25"/>
       <c r="C32" s="26"/>
       <c r="D32" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="18" t="s">
-        <v>25</v>
-      </c>
+      <c r="E32" s="29"/>
       <c r="F32" s="8">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="G32" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H32" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I32" s="22"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+    </row>
+    <row r="33" spans="2:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="B33" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G33" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H33" s="8">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="I33" s="23"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+    </row>
+    <row r="34" spans="2:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="B34" s="30"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H34" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I34" s="23"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+    </row>
+    <row r="35" spans="2:13" ht="63" x14ac:dyDescent="0.2">
+      <c r="B35" s="30"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="8">
         <v>0.78300000000000003</v>
       </c>
-      <c r="G32" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="H32" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="I32" s="35"/>
+      <c r="G35" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I35" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="I30:I32"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="I8:I11"/>
-    <mergeCell ref="I27:I29"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="I21:I23"/>
+  <mergeCells count="35">
     <mergeCell ref="E15:E17"/>
     <mergeCell ref="E18:E20"/>
     <mergeCell ref="B21:B23"/>
@@ -1674,6 +1729,32 @@
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="C18:C20"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="I33:I35"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="I8:I11"/>
+    <mergeCell ref="I27:I29"/>
+    <mergeCell ref="I21:I23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Experimented with more augmentation techniques
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yimenggu/Desktop/twitter-comms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A553DAD3-A5EB-3844-9446-2342DF2D263D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0747D88-7A96-5047-9973-F85F951436E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30900" yWindow="1460" windowWidth="28040" windowHeight="16200" activeTab="1" xr2:uid="{83E1EE90-11A9-2944-8CCC-8774B4B18D7B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="46">
   <si>
     <t>No.</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>ConDA(BLIP-2) w/ test_time_adaptation()  before validate() w/o triplet loss, using z as the input to the classifier instead of h</t>
+  </si>
+  <si>
+    <t>Difference between this setting and the above one: using random swap as the positive/augmentation</t>
+  </si>
+  <si>
+    <t>Difference between this setting and the above one: using random crop as the positive/augmentation</t>
   </si>
 </sst>
 </file>
@@ -365,47 +371,47 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -888,10 +894,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B38549D-5ACE-AD42-90AC-3551968574DA}">
-  <dimension ref="B3:M35"/>
+  <dimension ref="B3:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33:I35"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -935,10 +941,10 @@
       <c r="M3" s="13"/>
     </row>
     <row r="4" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="32" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="15" t="s">
@@ -956,15 +962,15 @@
       <c r="H4" s="8">
         <v>0.71699999999999997</v>
       </c>
-      <c r="I4" s="23"/>
+      <c r="I4" s="36"/>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
     </row>
     <row r="5" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B5" s="32"/>
-      <c r="C5" s="35"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="33"/>
       <c r="D5" s="17" t="s">
         <v>30</v>
       </c>
@@ -980,15 +986,15 @@
       <c r="H5" s="8">
         <v>0.80800000000000005</v>
       </c>
-      <c r="I5" s="23"/>
+      <c r="I5" s="36"/>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
     </row>
     <row r="6" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B6" s="32"/>
-      <c r="C6" s="35"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="33"/>
       <c r="D6" s="15" t="s">
         <v>31</v>
       </c>
@@ -1004,15 +1010,15 @@
       <c r="H6" s="8">
         <v>0.81100000000000005</v>
       </c>
-      <c r="I6" s="23"/>
+      <c r="I6" s="36"/>
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
     </row>
     <row r="7" spans="2:13" ht="21" x14ac:dyDescent="0.2">
-      <c r="B7" s="33"/>
-      <c r="C7" s="36"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="15" t="s">
         <v>23</v>
       </c>
@@ -1028,17 +1034,17 @@
       <c r="H7" s="8">
         <v>0.81100000000000005</v>
       </c>
-      <c r="I7" s="23"/>
+      <c r="I7" s="36"/>
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
       <c r="M7" s="13"/>
     </row>
     <row r="8" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="27" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="17" t="s">
@@ -1056,15 +1062,15 @@
       <c r="H8" s="8">
         <v>0.63700000000000001</v>
       </c>
-      <c r="I8" s="23"/>
+      <c r="I8" s="36"/>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
     </row>
     <row r="9" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B9" s="30"/>
-      <c r="C9" s="26"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="17" t="s">
         <v>30</v>
       </c>
@@ -1080,15 +1086,15 @@
       <c r="H9" s="8">
         <v>0.69299999999999995</v>
       </c>
-      <c r="I9" s="23"/>
+      <c r="I9" s="36"/>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
     </row>
     <row r="10" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B10" s="30"/>
-      <c r="C10" s="26"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="15" t="s">
         <v>31</v>
       </c>
@@ -1104,15 +1110,15 @@
       <c r="H10" s="8">
         <v>0.69799999999999995</v>
       </c>
-      <c r="I10" s="23"/>
+      <c r="I10" s="36"/>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
     </row>
     <row r="11" spans="2:13" ht="20" x14ac:dyDescent="0.2">
-      <c r="B11" s="30"/>
-      <c r="C11" s="26"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="19" t="s">
         <v>23</v>
       </c>
@@ -1128,17 +1134,17 @@
       <c r="H11" s="8">
         <v>0.69699999999999995</v>
       </c>
-      <c r="I11" s="23"/>
+      <c r="I11" s="36"/>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
     </row>
     <row r="12" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="27" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="17" t="s">
@@ -1156,15 +1162,15 @@
       <c r="H12" s="8">
         <v>0.72099999999999997</v>
       </c>
-      <c r="I12" s="23"/>
+      <c r="I12" s="36"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
     </row>
     <row r="13" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B13" s="30"/>
-      <c r="C13" s="26"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="17" t="s">
         <v>30</v>
       </c>
@@ -1180,15 +1186,15 @@
       <c r="H13" s="8">
         <v>0.76800000000000002</v>
       </c>
-      <c r="I13" s="23"/>
+      <c r="I13" s="36"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
     </row>
     <row r="14" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B14" s="30"/>
-      <c r="C14" s="26"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="15" t="s">
         <v>31</v>
       </c>
@@ -1204,23 +1210,23 @@
       <c r="H14" s="8">
         <v>0.77</v>
       </c>
-      <c r="I14" s="23"/>
+      <c r="I14" s="36"/>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
     </row>
     <row r="15" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="23">
         <v>1000</v>
       </c>
       <c r="F15" s="21" t="s">
@@ -1232,19 +1238,19 @@
       <c r="H15" s="8">
         <v>0.78400000000000003</v>
       </c>
-      <c r="I15" s="23"/>
+      <c r="I15" s="36"/>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
     </row>
     <row r="16" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B16" s="30"/>
-      <c r="C16" s="26"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="28"/>
+      <c r="E16" s="24"/>
       <c r="F16" s="21" t="s">
         <v>25</v>
       </c>
@@ -1254,19 +1260,19 @@
       <c r="H16" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="23"/>
+      <c r="I16" s="36"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
     </row>
     <row r="17" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B17" s="30"/>
-      <c r="C17" s="26"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="27"/>
       <c r="D17" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="29"/>
+      <c r="E17" s="25"/>
       <c r="F17" s="8">
         <v>0.80300000000000005</v>
       </c>
@@ -1276,23 +1282,23 @@
       <c r="H17" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="23"/>
+      <c r="I17" s="36"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
     </row>
     <row r="18" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="23">
         <v>1001</v>
       </c>
       <c r="F18" s="21" t="s">
@@ -1304,19 +1310,19 @@
       <c r="H18" s="8">
         <v>0.78500000000000003</v>
       </c>
-      <c r="I18" s="23"/>
+      <c r="I18" s="36"/>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
     </row>
     <row r="19" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B19" s="30"/>
-      <c r="C19" s="26"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="27"/>
       <c r="D19" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="28"/>
+      <c r="E19" s="24"/>
       <c r="F19" s="21" t="s">
         <v>25</v>
       </c>
@@ -1326,19 +1332,19 @@
       <c r="H19" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="23"/>
+      <c r="I19" s="36"/>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
     </row>
     <row r="20" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B20" s="30"/>
-      <c r="C20" s="26"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="29"/>
+      <c r="E20" s="25"/>
       <c r="F20" s="8">
         <v>0.80500000000000005</v>
       </c>
@@ -1348,23 +1354,23 @@
       <c r="H20" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="23"/>
+      <c r="I20" s="36"/>
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
       <c r="M20" s="13"/>
     </row>
     <row r="21" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="27">
+      <c r="E21" s="23">
         <v>1001</v>
       </c>
       <c r="F21" s="21" t="s">
@@ -1376,7 +1382,7 @@
       <c r="H21" s="8">
         <v>0.79300000000000004</v>
       </c>
-      <c r="I21" s="24" t="s">
+      <c r="I21" s="35" t="s">
         <v>40</v>
       </c>
       <c r="J21" s="13"/>
@@ -1385,12 +1391,12 @@
       <c r="M21" s="13"/>
     </row>
     <row r="22" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B22" s="25"/>
-      <c r="C22" s="26"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="28"/>
+      <c r="E22" s="24"/>
       <c r="F22" s="21" t="s">
         <v>25</v>
       </c>
@@ -1400,19 +1406,19 @@
       <c r="H22" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I22" s="24"/>
+      <c r="I22" s="35"/>
       <c r="J22" s="13"/>
       <c r="K22" s="13"/>
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>
     </row>
     <row r="23" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B23" s="25"/>
-      <c r="C23" s="26"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="29"/>
+      <c r="E23" s="25"/>
       <c r="F23" s="8">
         <v>0.80200000000000005</v>
       </c>
@@ -1422,23 +1428,23 @@
       <c r="H23" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I23" s="24"/>
+      <c r="I23" s="35"/>
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
       <c r="L23" s="13"/>
       <c r="M23" s="13"/>
     </row>
     <row r="24" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D24" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="27">
+      <c r="E24" s="23">
         <v>1001</v>
       </c>
       <c r="F24" s="21" t="s">
@@ -1450,19 +1456,19 @@
       <c r="H24" s="8">
         <v>0.78400000000000003</v>
       </c>
-      <c r="I24" s="24"/>
+      <c r="I24" s="35"/>
       <c r="J24" s="13"/>
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
       <c r="M24" s="13"/>
     </row>
     <row r="25" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B25" s="25"/>
-      <c r="C25" s="26"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="28"/>
+      <c r="E25" s="24"/>
       <c r="F25" s="21" t="s">
         <v>25</v>
       </c>
@@ -1472,19 +1478,19 @@
       <c r="H25" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I25" s="24"/>
+      <c r="I25" s="35"/>
       <c r="J25" s="13"/>
       <c r="K25" s="13"/>
       <c r="L25" s="13"/>
       <c r="M25" s="13"/>
     </row>
     <row r="26" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B26" s="25"/>
-      <c r="C26" s="26"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="29"/>
+      <c r="E26" s="25"/>
       <c r="F26" s="8">
         <v>0.80100000000000005</v>
       </c>
@@ -1494,23 +1500,23 @@
       <c r="H26" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I26" s="24"/>
+      <c r="I26" s="35"/>
       <c r="J26" s="13"/>
       <c r="K26" s="13"/>
       <c r="L26" s="13"/>
       <c r="M26" s="13"/>
     </row>
     <row r="27" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D27" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="27">
+      <c r="E27" s="23">
         <v>1001</v>
       </c>
       <c r="F27" s="21" t="s">
@@ -1522,7 +1528,7 @@
       <c r="H27" s="8">
         <v>0.79700000000000004</v>
       </c>
-      <c r="I27" s="24" t="s">
+      <c r="I27" s="35" t="s">
         <v>40</v>
       </c>
       <c r="J27" s="13"/>
@@ -1531,12 +1537,12 @@
       <c r="M27" s="13"/>
     </row>
     <row r="28" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B28" s="25"/>
-      <c r="C28" s="26"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="28"/>
+      <c r="E28" s="24"/>
       <c r="F28" s="21" t="s">
         <v>25</v>
       </c>
@@ -1546,19 +1552,19 @@
       <c r="H28" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I28" s="24"/>
+      <c r="I28" s="35"/>
       <c r="J28" s="13"/>
       <c r="K28" s="13"/>
       <c r="L28" s="13"/>
       <c r="M28" s="13"/>
     </row>
     <row r="29" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B29" s="25"/>
-      <c r="C29" s="26"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="27"/>
       <c r="D29" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="29"/>
+      <c r="E29" s="25"/>
       <c r="F29" s="8">
         <v>0.80300000000000005</v>
       </c>
@@ -1568,23 +1574,23 @@
       <c r="H29" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="24"/>
+      <c r="I29" s="35"/>
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
       <c r="L29" s="13"/>
       <c r="M29" s="13"/>
     </row>
     <row r="30" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B30" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="26" t="s">
+      <c r="B30" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E30" s="27">
+      <c r="E30" s="23">
         <v>1001</v>
       </c>
       <c r="F30" s="21" t="s">
@@ -1594,21 +1600,23 @@
         <v>25</v>
       </c>
       <c r="H30" s="8">
-        <v>0.79600000000000004</v>
-      </c>
-      <c r="I30" s="22"/>
+        <v>0.79900000000000004</v>
+      </c>
+      <c r="I30" s="35" t="s">
+        <v>44</v>
+      </c>
       <c r="J30" s="13"/>
       <c r="K30" s="13"/>
       <c r="L30" s="13"/>
       <c r="M30" s="13"/>
     </row>
     <row r="31" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B31" s="25"/>
-      <c r="C31" s="26"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="27"/>
       <c r="D31" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="28"/>
+      <c r="E31" s="24"/>
       <c r="F31" s="21" t="s">
         <v>25</v>
       </c>
@@ -1618,21 +1626,21 @@
       <c r="H31" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I31" s="22"/>
+      <c r="I31" s="35"/>
       <c r="J31" s="13"/>
       <c r="K31" s="13"/>
       <c r="L31" s="13"/>
       <c r="M31" s="13"/>
     </row>
     <row r="32" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B32" s="25"/>
-      <c r="C32" s="26"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="27"/>
       <c r="D32" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="29"/>
+      <c r="E32" s="25"/>
       <c r="F32" s="8">
-        <v>0.80100000000000005</v>
+        <v>0.8</v>
       </c>
       <c r="G32" s="21" t="s">
         <v>25</v>
@@ -1640,24 +1648,24 @@
       <c r="H32" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I32" s="22"/>
+      <c r="I32" s="35"/>
       <c r="J32" s="13"/>
       <c r="K32" s="13"/>
       <c r="L32" s="13"/>
       <c r="M32" s="13"/>
     </row>
     <row r="33" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B33" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33" s="26" t="s">
+      <c r="B33" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E33" s="18" t="s">
-        <v>25</v>
+      <c r="E33" s="23">
+        <v>1001</v>
       </c>
       <c r="F33" s="21" t="s">
         <v>25</v>
@@ -1666,60 +1674,240 @@
         <v>25</v>
       </c>
       <c r="H33" s="8">
-        <v>0.75600000000000001</v>
-      </c>
-      <c r="I33" s="23"/>
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="I33" s="35" t="s">
+        <v>45</v>
+      </c>
       <c r="J33" s="13"/>
       <c r="K33" s="13"/>
       <c r="L33" s="13"/>
       <c r="M33" s="13"/>
     </row>
     <row r="34" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B34" s="30"/>
-      <c r="C34" s="26"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E34" s="18" t="s">
-        <v>25</v>
-      </c>
+      <c r="E34" s="24"/>
       <c r="F34" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="G34" s="8" t="s">
-        <v>38</v>
+      <c r="G34" s="8">
+        <v>0.80500000000000005</v>
       </c>
       <c r="H34" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I34" s="23"/>
+      <c r="I34" s="35"/>
       <c r="J34" s="13"/>
       <c r="K34" s="13"/>
       <c r="L34" s="13"/>
       <c r="M34" s="13"/>
     </row>
     <row r="35" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B35" s="30"/>
-      <c r="C35" s="26"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="27"/>
       <c r="D35" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E35" s="18" t="s">
-        <v>25</v>
-      </c>
+      <c r="E35" s="25"/>
       <c r="F35" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="G35" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I35" s="35"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+    </row>
+    <row r="36" spans="2:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="B36" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="23">
+        <v>1001</v>
+      </c>
+      <c r="F36" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G36" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H36" s="8">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="I36" s="22"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+    </row>
+    <row r="37" spans="2:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="B37" s="26"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" s="24"/>
+      <c r="F37" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G37" s="8">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="H37" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I37" s="22"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+    </row>
+    <row r="38" spans="2:13" ht="63" x14ac:dyDescent="0.2">
+      <c r="B38" s="26"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E38" s="25"/>
+      <c r="F38" s="8">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="G38" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H38" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I38" s="22"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+    </row>
+    <row r="39" spans="2:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="B39" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G39" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H39" s="8">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="I39" s="36"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+    </row>
+    <row r="40" spans="2:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="B40" s="28"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H40" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I40" s="36"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+    </row>
+    <row r="41" spans="2:13" ht="63" x14ac:dyDescent="0.2">
+      <c r="B41" s="28"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" s="8">
         <v>0.78300000000000003</v>
       </c>
-      <c r="G35" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="H35" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="I35" s="23"/>
+      <c r="G41" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H41" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I41" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="43">
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="I33:I35"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="I39:I41"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="I8:I11"/>
+    <mergeCell ref="I27:I29"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I30:I32"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="B12:B14"/>
     <mergeCell ref="E15:E17"/>
     <mergeCell ref="E18:E20"/>
     <mergeCell ref="B21:B23"/>
@@ -1729,32 +1917,6 @@
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="C18:C20"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="I33:I35"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="I8:I11"/>
-    <mergeCell ref="I27:I29"/>
-    <mergeCell ref="I21:I23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated ConDA result on full training set
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yimenggu/Desktop/twitter-comms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985FA7AA-FDD5-6B46-8399-A3154341A690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BAA435-94C1-B441-AB15-68D2EA22F7BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33920" windowHeight="16100" activeTab="1" xr2:uid="{83E1EE90-11A9-2944-8CCC-8774B4B18D7B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" activeTab="1" xr2:uid="{83E1EE90-11A9-2944-8CCC-8774B4B18D7B}"/>
   </bookViews>
   <sheets>
     <sheet name="MLLMs" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="51">
   <si>
     <t>No.</t>
   </si>
@@ -404,6 +404,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -424,9 +427,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -909,10 +909,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B38549D-5ACE-AD42-90AC-3551968574DA}">
-  <dimension ref="B3:M53"/>
+  <dimension ref="B3:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42:I44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -956,10 +956,10 @@
       <c r="M3" s="13"/>
     </row>
     <row r="4" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="34" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="15" t="s">
@@ -977,15 +977,15 @@
       <c r="H4" s="8">
         <v>0.71699999999999997</v>
       </c>
-      <c r="I4" s="36"/>
+      <c r="I4" s="29"/>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
     </row>
     <row r="5" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B5" s="31"/>
-      <c r="C5" s="34"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="17" t="s">
         <v>30</v>
       </c>
@@ -1001,15 +1001,15 @@
       <c r="H5" s="8">
         <v>0.80800000000000005</v>
       </c>
-      <c r="I5" s="36"/>
+      <c r="I5" s="29"/>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
     </row>
     <row r="6" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B6" s="31"/>
-      <c r="C6" s="34"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="35"/>
       <c r="D6" s="15" t="s">
         <v>31</v>
       </c>
@@ -1025,15 +1025,15 @@
       <c r="H6" s="8">
         <v>0.81100000000000005</v>
       </c>
-      <c r="I6" s="36"/>
+      <c r="I6" s="29"/>
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
     </row>
     <row r="7" spans="2:13" ht="21" x14ac:dyDescent="0.2">
-      <c r="B7" s="32"/>
-      <c r="C7" s="35"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="36"/>
       <c r="D7" s="15" t="s">
         <v>23</v>
       </c>
@@ -1049,14 +1049,14 @@
       <c r="H7" s="8">
         <v>0.81100000000000005</v>
       </c>
-      <c r="I7" s="36"/>
+      <c r="I7" s="29"/>
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
       <c r="M7" s="13"/>
     </row>
     <row r="8" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="30" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -1077,14 +1077,14 @@
       <c r="H8" s="8">
         <v>0.63700000000000001</v>
       </c>
-      <c r="I8" s="36"/>
+      <c r="I8" s="29"/>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
     </row>
     <row r="9" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B9" s="29"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="24"/>
       <c r="D9" s="17" t="s">
         <v>30</v>
@@ -1101,14 +1101,14 @@
       <c r="H9" s="8">
         <v>0.69299999999999995</v>
       </c>
-      <c r="I9" s="36"/>
+      <c r="I9" s="29"/>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
     </row>
     <row r="10" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B10" s="29"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="24"/>
       <c r="D10" s="15" t="s">
         <v>31</v>
@@ -1125,14 +1125,14 @@
       <c r="H10" s="8">
         <v>0.69799999999999995</v>
       </c>
-      <c r="I10" s="36"/>
+      <c r="I10" s="29"/>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
     </row>
     <row r="11" spans="2:13" ht="20" x14ac:dyDescent="0.2">
-      <c r="B11" s="29"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="24"/>
       <c r="D11" s="19" t="s">
         <v>23</v>
@@ -1149,14 +1149,14 @@
       <c r="H11" s="8">
         <v>0.69699999999999995</v>
       </c>
-      <c r="I11" s="36"/>
+      <c r="I11" s="29"/>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
     </row>
     <row r="12" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="30" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="24" t="s">
@@ -1177,14 +1177,14 @@
       <c r="H12" s="8">
         <v>0.72099999999999997</v>
       </c>
-      <c r="I12" s="36"/>
+      <c r="I12" s="29"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
     </row>
     <row r="13" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B13" s="29"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="24"/>
       <c r="D13" s="17" t="s">
         <v>30</v>
@@ -1201,14 +1201,14 @@
       <c r="H13" s="8">
         <v>0.76800000000000002</v>
       </c>
-      <c r="I13" s="36"/>
+      <c r="I13" s="29"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
     </row>
     <row r="14" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B14" s="29"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="24"/>
       <c r="D14" s="15" t="s">
         <v>31</v>
@@ -1225,14 +1225,14 @@
       <c r="H14" s="8">
         <v>0.77</v>
       </c>
-      <c r="I14" s="36"/>
+      <c r="I14" s="29"/>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
     </row>
     <row r="15" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="30" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="24" t="s">
@@ -1253,14 +1253,14 @@
       <c r="H15" s="8">
         <v>0.78400000000000003</v>
       </c>
-      <c r="I15" s="36"/>
+      <c r="I15" s="29"/>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
     </row>
     <row r="16" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B16" s="29"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="24"/>
       <c r="D16" s="17" t="s">
         <v>30</v>
@@ -1275,14 +1275,14 @@
       <c r="H16" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="36"/>
+      <c r="I16" s="29"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
     </row>
     <row r="17" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B17" s="29"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="24"/>
       <c r="D17" s="15" t="s">
         <v>31</v>
@@ -1297,14 +1297,14 @@
       <c r="H17" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="36"/>
+      <c r="I17" s="29"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
     </row>
     <row r="18" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="30" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="24" t="s">
@@ -1325,14 +1325,14 @@
       <c r="H18" s="8">
         <v>0.78500000000000003</v>
       </c>
-      <c r="I18" s="36"/>
+      <c r="I18" s="29"/>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
     </row>
     <row r="19" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B19" s="29"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="24"/>
       <c r="D19" s="17" t="s">
         <v>30</v>
@@ -1347,14 +1347,14 @@
       <c r="H19" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="36"/>
+      <c r="I19" s="29"/>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
     </row>
     <row r="20" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B20" s="29"/>
+      <c r="B20" s="30"/>
       <c r="C20" s="24"/>
       <c r="D20" s="15" t="s">
         <v>31</v>
@@ -1369,7 +1369,7 @@
       <c r="H20" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="36"/>
+      <c r="I20" s="29"/>
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
@@ -2112,7 +2112,7 @@
       <c r="M50" s="13"/>
     </row>
     <row r="51" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B51" s="29" t="s">
+      <c r="B51" s="30" t="s">
         <v>22</v>
       </c>
       <c r="C51" s="24" t="s">
@@ -2133,14 +2133,14 @@
       <c r="H51" s="8">
         <v>0.75600000000000001</v>
       </c>
-      <c r="I51" s="36"/>
+      <c r="I51" s="29"/>
       <c r="J51" s="13"/>
       <c r="K51" s="13"/>
       <c r="L51" s="13"/>
       <c r="M51" s="13"/>
     </row>
     <row r="52" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B52" s="29"/>
+      <c r="B52" s="30"/>
       <c r="C52" s="24"/>
       <c r="D52" s="17" t="s">
         <v>30</v>
@@ -2157,14 +2157,14 @@
       <c r="H52" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I52" s="36"/>
+      <c r="I52" s="29"/>
       <c r="J52" s="13"/>
       <c r="K52" s="13"/>
       <c r="L52" s="13"/>
       <c r="M52" s="13"/>
     </row>
     <row r="53" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B53" s="29"/>
+      <c r="B53" s="30"/>
       <c r="C53" s="24"/>
       <c r="D53" s="15" t="s">
         <v>31</v>
@@ -2181,33 +2181,81 @@
       <c r="H53" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I53" s="36"/>
+      <c r="I53" s="29"/>
+    </row>
+    <row r="54" spans="2:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="B54" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D54" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E54" s="25">
+        <v>1001</v>
+      </c>
+      <c r="F54" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G54" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H54" s="8">
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="I54" s="28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" ht="42" x14ac:dyDescent="0.2">
+      <c r="B55" s="23"/>
+      <c r="C55" s="24"/>
+      <c r="D55" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E55" s="26"/>
+      <c r="F55" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G55" s="8">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="H55" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I55" s="28"/>
+    </row>
+    <row r="56" spans="2:13" ht="63" x14ac:dyDescent="0.2">
+      <c r="B56" s="23"/>
+      <c r="C56" s="24"/>
+      <c r="D56" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E56" s="27"/>
+      <c r="F56" s="8">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="G56" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H56" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I56" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="59">
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="E45:E47"/>
-    <mergeCell ref="I45:I47"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="I33:I35"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="I51:I53"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="I8:I11"/>
-    <mergeCell ref="I27:I29"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="I30:I32"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="I24:I26"/>
+  <mergeCells count="63">
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="E54:E56"/>
+    <mergeCell ref="I54:I56"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="B12:B14"/>
     <mergeCell ref="B51:B53"/>
     <mergeCell ref="C51:C53"/>
     <mergeCell ref="B27:B29"/>
@@ -2220,11 +2268,16 @@
     <mergeCell ref="C30:C32"/>
     <mergeCell ref="E30:E32"/>
     <mergeCell ref="B33:B35"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="E42:E44"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="E24:E26"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="C21:C23"/>
     <mergeCell ref="E21:E23"/>
@@ -2232,18 +2285,31 @@
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="E42:E44"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="I51:I53"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="I8:I11"/>
+    <mergeCell ref="I27:I29"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I30:I32"/>
+    <mergeCell ref="I24:I26"/>
     <mergeCell ref="I42:I44"/>
-    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="I36:I38"/>
+    <mergeCell ref="I39:I41"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="E45:E47"/>
+    <mergeCell ref="I45:I47"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="I33:I35"/>
     <mergeCell ref="C36:C38"/>
     <mergeCell ref="E36:E38"/>
-    <mergeCell ref="I36:I38"/>
     <mergeCell ref="B39:B41"/>
     <mergeCell ref="C39:C41"/>
     <mergeCell ref="E39:E41"/>
-    <mergeCell ref="I39:I41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Conducted some more experiments on NewsCLIPpings
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yimenggu/Desktop/twitter-comms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BAA435-94C1-B441-AB15-68D2EA22F7BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADF807E-20F5-264F-A133-4B5AA489700B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" activeTab="1" xr2:uid="{83E1EE90-11A9-2944-8CCC-8774B4B18D7B}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="28800" windowHeight="16100" activeTab="2" xr2:uid="{83E1EE90-11A9-2944-8CCC-8774B4B18D7B}"/>
   </bookViews>
   <sheets>
     <sheet name="MLLMs" sheetId="1" r:id="rId1"/>
-    <sheet name="ConDA" sheetId="2" r:id="rId2"/>
+    <sheet name="ConDA (Twitter-COMMs)" sheetId="2" r:id="rId2"/>
+    <sheet name="ConDA (NewsCLIPpings)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="67">
   <si>
     <t>No.</t>
   </si>
@@ -193,13 +194,65 @@
   </si>
   <si>
     <t>Difference between this setting and the above one: using synonym replacement and GaussianBlur as the positive/augmentation</t>
+  </si>
+  <si>
+    <t>On Twitter-COMMs</t>
+  </si>
+  <si>
+    <t>On NewsCLIPpings</t>
+  </si>
+  <si>
+    <t>Acc @ BBC</t>
+  </si>
+  <si>
+    <t>Acc @ Guardian</t>
+  </si>
+  <si>
+    <t>Acc @ USA Today</t>
+  </si>
+  <si>
+    <t>Acc @ Washington Post</t>
+  </si>
+  <si>
+    <t>Source: Guardian, USA Today, Washington Post
+Target: BBC</t>
+  </si>
+  <si>
+    <t>Source: BBC, USA Today, Washington Post
+Target: Guardian</t>
+  </si>
+  <si>
+    <t>Source: BBC, Guardian, Washington Post
+Target: USA Today</t>
+  </si>
+  <si>
+    <t>Source: BBC, Guardian, USA Today
+Target: Washington Post</t>
+  </si>
+  <si>
+    <t>Source: USA Today, Washington Post</t>
+  </si>
+  <si>
+    <t>Source: BBC, Guardian</t>
+  </si>
+  <si>
+    <t>Source: BBC</t>
+  </si>
+  <si>
+    <t>Source: USA Today</t>
+  </si>
+  <si>
+    <t>Source: Guardian</t>
+  </si>
+  <si>
+    <t>Source: Washington Post</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -220,8 +273,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,8 +311,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -322,11 +387,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -404,29 +482,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -909,10 +994,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B38549D-5ACE-AD42-90AC-3551968574DA}">
-  <dimension ref="B3:M56"/>
+  <dimension ref="B2:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -927,6 +1012,11 @@
     <col min="9" max="9" width="48.5" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:13" ht="20" x14ac:dyDescent="0.2">
+      <c r="B2" s="37" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="3" spans="2:13" ht="20" x14ac:dyDescent="0.2">
       <c r="B3" s="14" t="s">
         <v>18</v>
@@ -956,10 +1046,10 @@
       <c r="M3" s="13"/>
     </row>
     <row r="4" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="33" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="15" t="s">
@@ -977,15 +1067,15 @@
       <c r="H4" s="8">
         <v>0.71699999999999997</v>
       </c>
-      <c r="I4" s="29"/>
+      <c r="I4" s="36"/>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
     </row>
     <row r="5" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B5" s="32"/>
-      <c r="C5" s="35"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="34"/>
       <c r="D5" s="17" t="s">
         <v>30</v>
       </c>
@@ -1001,15 +1091,15 @@
       <c r="H5" s="8">
         <v>0.80800000000000005</v>
       </c>
-      <c r="I5" s="29"/>
+      <c r="I5" s="36"/>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
     </row>
     <row r="6" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B6" s="32"/>
-      <c r="C6" s="35"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="15" t="s">
         <v>31</v>
       </c>
@@ -1025,15 +1115,15 @@
       <c r="H6" s="8">
         <v>0.81100000000000005</v>
       </c>
-      <c r="I6" s="29"/>
+      <c r="I6" s="36"/>
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
     </row>
     <row r="7" spans="2:13" ht="21" x14ac:dyDescent="0.2">
-      <c r="B7" s="33"/>
-      <c r="C7" s="36"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="35"/>
       <c r="D7" s="15" t="s">
         <v>23</v>
       </c>
@@ -1049,14 +1139,14 @@
       <c r="H7" s="8">
         <v>0.81100000000000005</v>
       </c>
-      <c r="I7" s="29"/>
+      <c r="I7" s="36"/>
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
       <c r="M7" s="13"/>
     </row>
     <row r="8" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="29" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -1077,14 +1167,14 @@
       <c r="H8" s="8">
         <v>0.63700000000000001</v>
       </c>
-      <c r="I8" s="29"/>
+      <c r="I8" s="36"/>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
     </row>
     <row r="9" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B9" s="30"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="24"/>
       <c r="D9" s="17" t="s">
         <v>30</v>
@@ -1101,14 +1191,14 @@
       <c r="H9" s="8">
         <v>0.69299999999999995</v>
       </c>
-      <c r="I9" s="29"/>
+      <c r="I9" s="36"/>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
     </row>
     <row r="10" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B10" s="30"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="24"/>
       <c r="D10" s="15" t="s">
         <v>31</v>
@@ -1125,14 +1215,14 @@
       <c r="H10" s="8">
         <v>0.69799999999999995</v>
       </c>
-      <c r="I10" s="29"/>
+      <c r="I10" s="36"/>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
     </row>
     <row r="11" spans="2:13" ht="20" x14ac:dyDescent="0.2">
-      <c r="B11" s="30"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="24"/>
       <c r="D11" s="19" t="s">
         <v>23</v>
@@ -1149,14 +1239,14 @@
       <c r="H11" s="8">
         <v>0.69699999999999995</v>
       </c>
-      <c r="I11" s="29"/>
+      <c r="I11" s="36"/>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
     </row>
     <row r="12" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="29" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="24" t="s">
@@ -1177,14 +1267,14 @@
       <c r="H12" s="8">
         <v>0.72099999999999997</v>
       </c>
-      <c r="I12" s="29"/>
+      <c r="I12" s="36"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
     </row>
     <row r="13" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B13" s="30"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="24"/>
       <c r="D13" s="17" t="s">
         <v>30</v>
@@ -1201,14 +1291,14 @@
       <c r="H13" s="8">
         <v>0.76800000000000002</v>
       </c>
-      <c r="I13" s="29"/>
+      <c r="I13" s="36"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
     </row>
     <row r="14" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B14" s="30"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="24"/>
       <c r="D14" s="15" t="s">
         <v>31</v>
@@ -1225,14 +1315,14 @@
       <c r="H14" s="8">
         <v>0.77</v>
       </c>
-      <c r="I14" s="29"/>
+      <c r="I14" s="36"/>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
     </row>
     <row r="15" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="29" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="24" t="s">
@@ -1253,14 +1343,14 @@
       <c r="H15" s="8">
         <v>0.78400000000000003</v>
       </c>
-      <c r="I15" s="29"/>
+      <c r="I15" s="36"/>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
     </row>
     <row r="16" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B16" s="30"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="24"/>
       <c r="D16" s="17" t="s">
         <v>30</v>
@@ -1275,14 +1365,14 @@
       <c r="H16" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="29"/>
+      <c r="I16" s="36"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
     </row>
     <row r="17" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B17" s="30"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="24"/>
       <c r="D17" s="15" t="s">
         <v>31</v>
@@ -1297,14 +1387,14 @@
       <c r="H17" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="29"/>
+      <c r="I17" s="36"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
     </row>
     <row r="18" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="29" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="24" t="s">
@@ -1325,14 +1415,14 @@
       <c r="H18" s="8">
         <v>0.78500000000000003</v>
       </c>
-      <c r="I18" s="29"/>
+      <c r="I18" s="36"/>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
     </row>
     <row r="19" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B19" s="30"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="24"/>
       <c r="D19" s="17" t="s">
         <v>30</v>
@@ -1347,14 +1437,14 @@
       <c r="H19" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="29"/>
+      <c r="I19" s="36"/>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
     </row>
     <row r="20" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B20" s="30"/>
+      <c r="B20" s="29"/>
       <c r="C20" s="24"/>
       <c r="D20" s="15" t="s">
         <v>31</v>
@@ -1369,7 +1459,7 @@
       <c r="H20" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="29"/>
+      <c r="I20" s="36"/>
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
@@ -2112,7 +2202,7 @@
       <c r="M50" s="13"/>
     </row>
     <row r="51" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B51" s="30" t="s">
+      <c r="B51" s="29" t="s">
         <v>22</v>
       </c>
       <c r="C51" s="24" t="s">
@@ -2133,14 +2223,14 @@
       <c r="H51" s="8">
         <v>0.75600000000000001</v>
       </c>
-      <c r="I51" s="29"/>
+      <c r="I51" s="36"/>
       <c r="J51" s="13"/>
       <c r="K51" s="13"/>
       <c r="L51" s="13"/>
       <c r="M51" s="13"/>
     </row>
     <row r="52" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B52" s="30"/>
+      <c r="B52" s="29"/>
       <c r="C52" s="24"/>
       <c r="D52" s="17" t="s">
         <v>30</v>
@@ -2157,14 +2247,14 @@
       <c r="H52" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I52" s="29"/>
+      <c r="I52" s="36"/>
       <c r="J52" s="13"/>
       <c r="K52" s="13"/>
       <c r="L52" s="13"/>
       <c r="M52" s="13"/>
     </row>
     <row r="53" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B53" s="30"/>
+      <c r="B53" s="29"/>
       <c r="C53" s="24"/>
       <c r="D53" s="15" t="s">
         <v>31</v>
@@ -2181,7 +2271,7 @@
       <c r="H53" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I53" s="29"/>
+      <c r="I53" s="36"/>
     </row>
     <row r="54" spans="2:13" ht="42" x14ac:dyDescent="0.2">
       <c r="B54" s="23" t="s">
@@ -2247,44 +2337,18 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="C54:C56"/>
-    <mergeCell ref="E54:E56"/>
-    <mergeCell ref="I54:I56"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B51:B53"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="C48:C50"/>
-    <mergeCell ref="E48:E50"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="E42:E44"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="E45:E47"/>
+    <mergeCell ref="I45:I47"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="I33:I35"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="E39:E41"/>
     <mergeCell ref="I4:I7"/>
     <mergeCell ref="I51:I53"/>
     <mergeCell ref="I18:I20"/>
@@ -2298,19 +2362,330 @@
     <mergeCell ref="I42:I44"/>
     <mergeCell ref="I36:I38"/>
     <mergeCell ref="I39:I41"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="E45:E47"/>
-    <mergeCell ref="I45:I47"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="I33:I35"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="E54:E56"/>
+    <mergeCell ref="I54:I56"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="E48:E50"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="E42:E44"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="B21:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB266944-C992-CA4E-B72E-F8C46C08F0CD}">
+  <dimension ref="B2:I13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="31.83203125" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" customWidth="1"/>
+    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="8" max="8" width="24" customWidth="1"/>
+    <col min="9" max="9" width="29.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="20" x14ac:dyDescent="0.2">
+      <c r="B2" s="37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" ht="20" x14ac:dyDescent="0.2">
+      <c r="B3" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="39">
+        <v>0.7036</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0.76070000000000004</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0.82140000000000002</v>
+      </c>
+      <c r="I4" s="8">
+        <v>0.78339999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="29"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0.73219999999999996</v>
+      </c>
+      <c r="G5" s="39">
+        <v>0.74880000000000002</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0.81810000000000005</v>
+      </c>
+      <c r="I5" s="8">
+        <v>0.78200000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="29"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0.73260000000000003</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0.76</v>
+      </c>
+      <c r="H6" s="39">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="I6" s="8">
+        <v>0.77649999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="29"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.72550000000000003</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="H7" s="8">
+        <v>0.81520000000000004</v>
+      </c>
+      <c r="I7" s="39">
+        <v>0.77580000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="74" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="29"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="39">
+        <v>0.67120000000000002</v>
+      </c>
+      <c r="G8" s="39">
+        <v>0.73419999999999996</v>
+      </c>
+      <c r="H8" s="8">
+        <v>0.82820000000000005</v>
+      </c>
+      <c r="I8" s="8">
+        <v>0.78790000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="B9" s="29"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.7319</v>
+      </c>
+      <c r="G9" s="8">
+        <v>0.7601</v>
+      </c>
+      <c r="H9" s="39">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="I9" s="39">
+        <v>0.76590000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="B10" s="29"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.75309999999999999</v>
+      </c>
+      <c r="G10" s="39">
+        <v>0.73009999999999997</v>
+      </c>
+      <c r="H10" s="39">
+        <v>0.75270000000000004</v>
+      </c>
+      <c r="I10" s="39">
+        <v>0.7399</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="B11" s="29"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="39">
+        <v>0.6784</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0.7339</v>
+      </c>
+      <c r="H11" s="39">
+        <v>0.81659999999999999</v>
+      </c>
+      <c r="I11" s="39">
+        <v>0.78920000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="B12" s="29"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="39">
+        <v>0.65759999999999996</v>
+      </c>
+      <c r="G12" s="39">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="H12" s="8">
+        <v>0.82820000000000005</v>
+      </c>
+      <c r="I12" s="39">
+        <v>0.77759999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="B13" s="29"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="39">
+        <v>0.68079999999999996</v>
+      </c>
+      <c r="G13" s="39">
+        <v>0.73560000000000003</v>
+      </c>
+      <c r="H13" s="39">
+        <v>0.81589999999999996</v>
+      </c>
+      <c r="I13" s="8">
+        <v>0.78810000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C4:C13"/>
+    <mergeCell ref="B4:B13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Corrected the tensor used
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yimenggu/Desktop/twitter-comms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADF807E-20F5-264F-A133-4B5AA489700B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BCB587-5F0C-DB4E-B5A4-5FBF920C23D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="28800" windowHeight="16100" activeTab="2" xr2:uid="{83E1EE90-11A9-2944-8CCC-8774B4B18D7B}"/>
+    <workbookView xWindow="28800" yWindow="560" windowWidth="28800" windowHeight="16100" activeTab="2" xr2:uid="{83E1EE90-11A9-2944-8CCC-8774B4B18D7B}"/>
   </bookViews>
   <sheets>
     <sheet name="MLLMs" sheetId="1" r:id="rId1"/>
@@ -464,54 +464,54 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1013,7 +1013,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="20" x14ac:dyDescent="0.2">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="23" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1046,10 +1046,10 @@
       <c r="M3" s="13"/>
     </row>
     <row r="4" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="37" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="15" t="s">
@@ -1067,15 +1067,15 @@
       <c r="H4" s="8">
         <v>0.71699999999999997</v>
       </c>
-      <c r="I4" s="36"/>
+      <c r="I4" s="32"/>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
     </row>
     <row r="5" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B5" s="31"/>
-      <c r="C5" s="34"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="17" t="s">
         <v>30</v>
       </c>
@@ -1091,15 +1091,15 @@
       <c r="H5" s="8">
         <v>0.80800000000000005</v>
       </c>
-      <c r="I5" s="36"/>
+      <c r="I5" s="32"/>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
     </row>
     <row r="6" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B6" s="31"/>
-      <c r="C6" s="34"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="38"/>
       <c r="D6" s="15" t="s">
         <v>31</v>
       </c>
@@ -1115,15 +1115,15 @@
       <c r="H6" s="8">
         <v>0.81100000000000005</v>
       </c>
-      <c r="I6" s="36"/>
+      <c r="I6" s="32"/>
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
     </row>
     <row r="7" spans="2:13" ht="21" x14ac:dyDescent="0.2">
-      <c r="B7" s="32"/>
-      <c r="C7" s="35"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="39"/>
       <c r="D7" s="15" t="s">
         <v>23</v>
       </c>
@@ -1139,17 +1139,17 @@
       <c r="H7" s="8">
         <v>0.81100000000000005</v>
       </c>
-      <c r="I7" s="36"/>
+      <c r="I7" s="32"/>
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
       <c r="M7" s="13"/>
     </row>
     <row r="8" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="27" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="17" t="s">
@@ -1167,15 +1167,15 @@
       <c r="H8" s="8">
         <v>0.63700000000000001</v>
       </c>
-      <c r="I8" s="36"/>
+      <c r="I8" s="32"/>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
     </row>
     <row r="9" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B9" s="29"/>
-      <c r="C9" s="24"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="17" t="s">
         <v>30</v>
       </c>
@@ -1191,15 +1191,15 @@
       <c r="H9" s="8">
         <v>0.69299999999999995</v>
       </c>
-      <c r="I9" s="36"/>
+      <c r="I9" s="32"/>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
     </row>
     <row r="10" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B10" s="29"/>
-      <c r="C10" s="24"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="15" t="s">
         <v>31</v>
       </c>
@@ -1215,15 +1215,15 @@
       <c r="H10" s="8">
         <v>0.69799999999999995</v>
       </c>
-      <c r="I10" s="36"/>
+      <c r="I10" s="32"/>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
     </row>
     <row r="11" spans="2:13" ht="20" x14ac:dyDescent="0.2">
-      <c r="B11" s="29"/>
-      <c r="C11" s="24"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="19" t="s">
         <v>23</v>
       </c>
@@ -1239,17 +1239,17 @@
       <c r="H11" s="8">
         <v>0.69699999999999995</v>
       </c>
-      <c r="I11" s="36"/>
+      <c r="I11" s="32"/>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
     </row>
     <row r="12" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="27" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="17" t="s">
@@ -1267,15 +1267,15 @@
       <c r="H12" s="8">
         <v>0.72099999999999997</v>
       </c>
-      <c r="I12" s="36"/>
+      <c r="I12" s="32"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
     </row>
     <row r="13" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B13" s="29"/>
-      <c r="C13" s="24"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="17" t="s">
         <v>30</v>
       </c>
@@ -1291,15 +1291,15 @@
       <c r="H13" s="8">
         <v>0.76800000000000002</v>
       </c>
-      <c r="I13" s="36"/>
+      <c r="I13" s="32"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
     </row>
     <row r="14" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B14" s="29"/>
-      <c r="C14" s="24"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="15" t="s">
         <v>31</v>
       </c>
@@ -1315,23 +1315,23 @@
       <c r="H14" s="8">
         <v>0.77</v>
       </c>
-      <c r="I14" s="36"/>
+      <c r="I14" s="32"/>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
     </row>
     <row r="15" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="28">
         <v>1000</v>
       </c>
       <c r="F15" s="21" t="s">
@@ -1343,19 +1343,19 @@
       <c r="H15" s="8">
         <v>0.78400000000000003</v>
       </c>
-      <c r="I15" s="36"/>
+      <c r="I15" s="32"/>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
     </row>
     <row r="16" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B16" s="29"/>
-      <c r="C16" s="24"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="26"/>
+      <c r="E16" s="29"/>
       <c r="F16" s="21" t="s">
         <v>25</v>
       </c>
@@ -1365,19 +1365,19 @@
       <c r="H16" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="36"/>
+      <c r="I16" s="32"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
     </row>
     <row r="17" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B17" s="29"/>
-      <c r="C17" s="24"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="27"/>
       <c r="D17" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="27"/>
+      <c r="E17" s="30"/>
       <c r="F17" s="8">
         <v>0.80300000000000005</v>
       </c>
@@ -1387,23 +1387,23 @@
       <c r="H17" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="36"/>
+      <c r="I17" s="32"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
     </row>
     <row r="18" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="25">
+      <c r="E18" s="28">
         <v>1001</v>
       </c>
       <c r="F18" s="21" t="s">
@@ -1415,19 +1415,19 @@
       <c r="H18" s="8">
         <v>0.78500000000000003</v>
       </c>
-      <c r="I18" s="36"/>
+      <c r="I18" s="32"/>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
     </row>
     <row r="19" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B19" s="29"/>
-      <c r="C19" s="24"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="27"/>
       <c r="D19" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="26"/>
+      <c r="E19" s="29"/>
       <c r="F19" s="21" t="s">
         <v>25</v>
       </c>
@@ -1437,19 +1437,19 @@
       <c r="H19" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="36"/>
+      <c r="I19" s="32"/>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
     </row>
     <row r="20" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B20" s="29"/>
-      <c r="C20" s="24"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="27"/>
+      <c r="E20" s="30"/>
       <c r="F20" s="8">
         <v>0.80500000000000005</v>
       </c>
@@ -1459,23 +1459,23 @@
       <c r="H20" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="36"/>
+      <c r="I20" s="32"/>
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
       <c r="M20" s="13"/>
     </row>
     <row r="21" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E21" s="28">
         <v>1001</v>
       </c>
       <c r="F21" s="21" t="s">
@@ -1487,7 +1487,7 @@
       <c r="H21" s="8">
         <v>0.79300000000000004</v>
       </c>
-      <c r="I21" s="28" t="s">
+      <c r="I21" s="31" t="s">
         <v>40</v>
       </c>
       <c r="J21" s="13"/>
@@ -1496,12 +1496,12 @@
       <c r="M21" s="13"/>
     </row>
     <row r="22" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B22" s="23"/>
-      <c r="C22" s="24"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="26"/>
+      <c r="E22" s="29"/>
       <c r="F22" s="21" t="s">
         <v>25</v>
       </c>
@@ -1511,19 +1511,19 @@
       <c r="H22" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I22" s="28"/>
+      <c r="I22" s="31"/>
       <c r="J22" s="13"/>
       <c r="K22" s="13"/>
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>
     </row>
     <row r="23" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B23" s="23"/>
-      <c r="C23" s="24"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="27"/>
+      <c r="E23" s="30"/>
       <c r="F23" s="8">
         <v>0.80200000000000005</v>
       </c>
@@ -1533,23 +1533,23 @@
       <c r="H23" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I23" s="28"/>
+      <c r="I23" s="31"/>
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
       <c r="L23" s="13"/>
       <c r="M23" s="13"/>
     </row>
     <row r="24" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D24" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24" s="28">
         <v>1001</v>
       </c>
       <c r="F24" s="21" t="s">
@@ -1561,19 +1561,19 @@
       <c r="H24" s="8">
         <v>0.78400000000000003</v>
       </c>
-      <c r="I24" s="28"/>
+      <c r="I24" s="31"/>
       <c r="J24" s="13"/>
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
       <c r="M24" s="13"/>
     </row>
     <row r="25" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B25" s="23"/>
-      <c r="C25" s="24"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="26"/>
+      <c r="E25" s="29"/>
       <c r="F25" s="21" t="s">
         <v>25</v>
       </c>
@@ -1583,19 +1583,19 @@
       <c r="H25" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I25" s="28"/>
+      <c r="I25" s="31"/>
       <c r="J25" s="13"/>
       <c r="K25" s="13"/>
       <c r="L25" s="13"/>
       <c r="M25" s="13"/>
     </row>
     <row r="26" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B26" s="23"/>
-      <c r="C26" s="24"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="27"/>
+      <c r="E26" s="30"/>
       <c r="F26" s="8">
         <v>0.80100000000000005</v>
       </c>
@@ -1605,23 +1605,23 @@
       <c r="H26" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I26" s="28"/>
+      <c r="I26" s="31"/>
       <c r="J26" s="13"/>
       <c r="K26" s="13"/>
       <c r="L26" s="13"/>
       <c r="M26" s="13"/>
     </row>
     <row r="27" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D27" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="25">
+      <c r="E27" s="28">
         <v>1001</v>
       </c>
       <c r="F27" s="21" t="s">
@@ -1633,7 +1633,7 @@
       <c r="H27" s="8">
         <v>0.79700000000000004</v>
       </c>
-      <c r="I27" s="28" t="s">
+      <c r="I27" s="31" t="s">
         <v>49</v>
       </c>
       <c r="J27" s="13"/>
@@ -1642,12 +1642,12 @@
       <c r="M27" s="13"/>
     </row>
     <row r="28" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B28" s="23"/>
-      <c r="C28" s="24"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="26"/>
+      <c r="E28" s="29"/>
       <c r="F28" s="21" t="s">
         <v>25</v>
       </c>
@@ -1657,19 +1657,19 @@
       <c r="H28" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I28" s="28"/>
+      <c r="I28" s="31"/>
       <c r="J28" s="13"/>
       <c r="K28" s="13"/>
       <c r="L28" s="13"/>
       <c r="M28" s="13"/>
     </row>
     <row r="29" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B29" s="23"/>
-      <c r="C29" s="24"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="27"/>
       <c r="D29" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="27"/>
+      <c r="E29" s="30"/>
       <c r="F29" s="8">
         <v>0.80300000000000005</v>
       </c>
@@ -1679,23 +1679,23 @@
       <c r="H29" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="28"/>
+      <c r="I29" s="31"/>
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
       <c r="L29" s="13"/>
       <c r="M29" s="13"/>
     </row>
     <row r="30" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="24" t="s">
+      <c r="C30" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E30" s="25">
+      <c r="E30" s="28">
         <v>1001</v>
       </c>
       <c r="F30" s="21" t="s">
@@ -1707,7 +1707,7 @@
       <c r="H30" s="8">
         <v>0.79900000000000004</v>
       </c>
-      <c r="I30" s="28" t="s">
+      <c r="I30" s="31" t="s">
         <v>44</v>
       </c>
       <c r="J30" s="13"/>
@@ -1716,12 +1716,12 @@
       <c r="M30" s="13"/>
     </row>
     <row r="31" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B31" s="23"/>
-      <c r="C31" s="24"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="27"/>
       <c r="D31" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="26"/>
+      <c r="E31" s="29"/>
       <c r="F31" s="21" t="s">
         <v>25</v>
       </c>
@@ -1731,19 +1731,19 @@
       <c r="H31" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I31" s="28"/>
+      <c r="I31" s="31"/>
       <c r="J31" s="13"/>
       <c r="K31" s="13"/>
       <c r="L31" s="13"/>
       <c r="M31" s="13"/>
     </row>
     <row r="32" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B32" s="23"/>
-      <c r="C32" s="24"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="27"/>
       <c r="D32" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="27"/>
+      <c r="E32" s="30"/>
       <c r="F32" s="8">
         <v>0.8</v>
       </c>
@@ -1753,23 +1753,23 @@
       <c r="H32" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I32" s="28"/>
+      <c r="I32" s="31"/>
       <c r="J32" s="13"/>
       <c r="K32" s="13"/>
       <c r="L32" s="13"/>
       <c r="M32" s="13"/>
     </row>
     <row r="33" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="24" t="s">
+      <c r="C33" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E33" s="25">
+      <c r="E33" s="28">
         <v>1001</v>
       </c>
       <c r="F33" s="21" t="s">
@@ -1781,7 +1781,7 @@
       <c r="H33" s="8">
         <v>0.79300000000000004</v>
       </c>
-      <c r="I33" s="28" t="s">
+      <c r="I33" s="31" t="s">
         <v>45</v>
       </c>
       <c r="J33" s="13"/>
@@ -1790,12 +1790,12 @@
       <c r="M33" s="13"/>
     </row>
     <row r="34" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B34" s="23"/>
-      <c r="C34" s="24"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E34" s="26"/>
+      <c r="E34" s="29"/>
       <c r="F34" s="21" t="s">
         <v>25</v>
       </c>
@@ -1805,19 +1805,19 @@
       <c r="H34" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I34" s="28"/>
+      <c r="I34" s="31"/>
       <c r="J34" s="13"/>
       <c r="K34" s="13"/>
       <c r="L34" s="13"/>
       <c r="M34" s="13"/>
     </row>
     <row r="35" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B35" s="23"/>
-      <c r="C35" s="24"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="27"/>
       <c r="D35" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E35" s="27"/>
+      <c r="E35" s="30"/>
       <c r="F35" s="8">
         <v>0.8</v>
       </c>
@@ -1827,23 +1827,23 @@
       <c r="H35" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I35" s="28"/>
+      <c r="I35" s="31"/>
       <c r="J35" s="13"/>
       <c r="K35" s="13"/>
       <c r="L35" s="13"/>
       <c r="M35" s="13"/>
     </row>
     <row r="36" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B36" s="23" t="s">
+      <c r="B36" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D36" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E36" s="25">
+      <c r="E36" s="28">
         <v>1001</v>
       </c>
       <c r="F36" s="21" t="s">
@@ -1855,7 +1855,7 @@
       <c r="H36" s="8">
         <v>0.79400000000000004</v>
       </c>
-      <c r="I36" s="28" t="s">
+      <c r="I36" s="31" t="s">
         <v>46</v>
       </c>
       <c r="J36" s="13"/>
@@ -1864,12 +1864,12 @@
       <c r="M36" s="13"/>
     </row>
     <row r="37" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B37" s="23"/>
-      <c r="C37" s="24"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="27"/>
       <c r="D37" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E37" s="26"/>
+      <c r="E37" s="29"/>
       <c r="F37" s="21" t="s">
         <v>25</v>
       </c>
@@ -1879,19 +1879,19 @@
       <c r="H37" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I37" s="28"/>
+      <c r="I37" s="31"/>
       <c r="J37" s="13"/>
       <c r="K37" s="13"/>
       <c r="L37" s="13"/>
       <c r="M37" s="13"/>
     </row>
     <row r="38" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B38" s="23"/>
-      <c r="C38" s="24"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="27"/>
       <c r="D38" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E38" s="27"/>
+      <c r="E38" s="30"/>
       <c r="F38" s="8">
         <v>0.8</v>
       </c>
@@ -1901,23 +1901,23 @@
       <c r="H38" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I38" s="28"/>
+      <c r="I38" s="31"/>
       <c r="J38" s="13"/>
       <c r="K38" s="13"/>
       <c r="L38" s="13"/>
       <c r="M38" s="13"/>
     </row>
     <row r="39" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D39" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E39" s="25">
+      <c r="E39" s="28">
         <v>1001</v>
       </c>
       <c r="F39" s="21" t="s">
@@ -1929,7 +1929,7 @@
       <c r="H39" s="8">
         <v>0.80100000000000005</v>
       </c>
-      <c r="I39" s="28" t="s">
+      <c r="I39" s="31" t="s">
         <v>47</v>
       </c>
       <c r="J39" s="13"/>
@@ -1938,12 +1938,12 @@
       <c r="M39" s="13"/>
     </row>
     <row r="40" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B40" s="23"/>
-      <c r="C40" s="24"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="27"/>
       <c r="D40" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E40" s="26"/>
+      <c r="E40" s="29"/>
       <c r="F40" s="21" t="s">
         <v>25</v>
       </c>
@@ -1953,19 +1953,19 @@
       <c r="H40" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I40" s="28"/>
+      <c r="I40" s="31"/>
       <c r="J40" s="13"/>
       <c r="K40" s="13"/>
       <c r="L40" s="13"/>
       <c r="M40" s="13"/>
     </row>
     <row r="41" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B41" s="23"/>
-      <c r="C41" s="24"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="27"/>
       <c r="D41" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E41" s="27"/>
+      <c r="E41" s="30"/>
       <c r="F41" s="8">
         <v>0.79900000000000004</v>
       </c>
@@ -1975,23 +1975,23 @@
       <c r="H41" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I41" s="28"/>
+      <c r="I41" s="31"/>
       <c r="J41" s="13"/>
       <c r="K41" s="13"/>
       <c r="L41" s="13"/>
       <c r="M41" s="13"/>
     </row>
     <row r="42" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B42" s="23" t="s">
+      <c r="B42" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="24" t="s">
+      <c r="C42" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D42" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E42" s="25">
+      <c r="E42" s="28">
         <v>1001</v>
       </c>
       <c r="F42" s="21" t="s">
@@ -2003,7 +2003,7 @@
       <c r="H42" s="8">
         <v>0.8</v>
       </c>
-      <c r="I42" s="28" t="s">
+      <c r="I42" s="31" t="s">
         <v>48</v>
       </c>
       <c r="J42" s="13"/>
@@ -2012,12 +2012,12 @@
       <c r="M42" s="13"/>
     </row>
     <row r="43" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B43" s="23"/>
-      <c r="C43" s="24"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="27"/>
       <c r="D43" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E43" s="26"/>
+      <c r="E43" s="29"/>
       <c r="F43" s="21" t="s">
         <v>25</v>
       </c>
@@ -2027,19 +2027,19 @@
       <c r="H43" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I43" s="28"/>
+      <c r="I43" s="31"/>
       <c r="J43" s="13"/>
       <c r="K43" s="13"/>
       <c r="L43" s="13"/>
       <c r="M43" s="13"/>
     </row>
     <row r="44" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B44" s="23"/>
-      <c r="C44" s="24"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="27"/>
       <c r="D44" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E44" s="27"/>
+      <c r="E44" s="30"/>
       <c r="F44" s="8">
         <v>0.80100000000000005</v>
       </c>
@@ -2049,23 +2049,23 @@
       <c r="H44" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I44" s="28"/>
+      <c r="I44" s="31"/>
       <c r="J44" s="13"/>
       <c r="K44" s="13"/>
       <c r="L44" s="13"/>
       <c r="M44" s="13"/>
     </row>
     <row r="45" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B45" s="23" t="s">
+      <c r="B45" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C45" s="24" t="s">
+      <c r="C45" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D45" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E45" s="25">
+      <c r="E45" s="28">
         <v>1001</v>
       </c>
       <c r="F45" s="21" t="s">
@@ -2077,7 +2077,7 @@
       <c r="H45" s="8">
         <v>0.79500000000000004</v>
       </c>
-      <c r="I45" s="28" t="s">
+      <c r="I45" s="31" t="s">
         <v>50</v>
       </c>
       <c r="J45" s="13"/>
@@ -2086,12 +2086,12 @@
       <c r="M45" s="13"/>
     </row>
     <row r="46" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B46" s="23"/>
-      <c r="C46" s="24"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="27"/>
       <c r="D46" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E46" s="26"/>
+      <c r="E46" s="29"/>
       <c r="F46" s="21" t="s">
         <v>25</v>
       </c>
@@ -2101,19 +2101,19 @@
       <c r="H46" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I46" s="28"/>
+      <c r="I46" s="31"/>
       <c r="J46" s="13"/>
       <c r="K46" s="13"/>
       <c r="L46" s="13"/>
       <c r="M46" s="13"/>
     </row>
     <row r="47" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B47" s="23"/>
-      <c r="C47" s="24"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="27"/>
       <c r="D47" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E47" s="27"/>
+      <c r="E47" s="30"/>
       <c r="F47" s="8">
         <v>0.80500000000000005</v>
       </c>
@@ -2123,23 +2123,23 @@
       <c r="H47" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I47" s="28"/>
+      <c r="I47" s="31"/>
       <c r="J47" s="13"/>
       <c r="K47" s="13"/>
       <c r="L47" s="13"/>
       <c r="M47" s="13"/>
     </row>
     <row r="48" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B48" s="23" t="s">
+      <c r="B48" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="C48" s="24" t="s">
+      <c r="C48" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D48" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E48" s="25">
+      <c r="E48" s="28">
         <v>1001</v>
       </c>
       <c r="F48" s="21" t="s">
@@ -2158,12 +2158,12 @@
       <c r="M48" s="13"/>
     </row>
     <row r="49" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B49" s="23"/>
-      <c r="C49" s="24"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="27"/>
       <c r="D49" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E49" s="26"/>
+      <c r="E49" s="29"/>
       <c r="F49" s="21" t="s">
         <v>25</v>
       </c>
@@ -2180,12 +2180,12 @@
       <c r="M49" s="13"/>
     </row>
     <row r="50" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B50" s="23"/>
-      <c r="C50" s="24"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="27"/>
       <c r="D50" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E50" s="27"/>
+      <c r="E50" s="30"/>
       <c r="F50" s="8">
         <v>0.80100000000000005</v>
       </c>
@@ -2202,10 +2202,10 @@
       <c r="M50" s="13"/>
     </row>
     <row r="51" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B51" s="29" t="s">
+      <c r="B51" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="C51" s="24" t="s">
+      <c r="C51" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D51" s="17" t="s">
@@ -2223,15 +2223,15 @@
       <c r="H51" s="8">
         <v>0.75600000000000001</v>
       </c>
-      <c r="I51" s="36"/>
+      <c r="I51" s="32"/>
       <c r="J51" s="13"/>
       <c r="K51" s="13"/>
       <c r="L51" s="13"/>
       <c r="M51" s="13"/>
     </row>
     <row r="52" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B52" s="29"/>
-      <c r="C52" s="24"/>
+      <c r="B52" s="33"/>
+      <c r="C52" s="27"/>
       <c r="D52" s="17" t="s">
         <v>30</v>
       </c>
@@ -2247,15 +2247,15 @@
       <c r="H52" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I52" s="36"/>
+      <c r="I52" s="32"/>
       <c r="J52" s="13"/>
       <c r="K52" s="13"/>
       <c r="L52" s="13"/>
       <c r="M52" s="13"/>
     </row>
     <row r="53" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B53" s="29"/>
-      <c r="C53" s="24"/>
+      <c r="B53" s="33"/>
+      <c r="C53" s="27"/>
       <c r="D53" s="15" t="s">
         <v>31</v>
       </c>
@@ -2271,19 +2271,19 @@
       <c r="H53" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I53" s="36"/>
+      <c r="I53" s="32"/>
     </row>
     <row r="54" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B54" s="23" t="s">
+      <c r="B54" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C54" s="24" t="s">
+      <c r="C54" s="27" t="s">
         <v>24</v>
       </c>
       <c r="D54" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E54" s="25">
+      <c r="E54" s="28">
         <v>1001</v>
       </c>
       <c r="F54" s="21" t="s">
@@ -2295,17 +2295,17 @@
       <c r="H54" s="8">
         <v>0.79300000000000004</v>
       </c>
-      <c r="I54" s="28" t="s">
+      <c r="I54" s="31" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="55" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B55" s="23"/>
-      <c r="C55" s="24"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="27"/>
       <c r="D55" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E55" s="26"/>
+      <c r="E55" s="29"/>
       <c r="F55" s="21" t="s">
         <v>25</v>
       </c>
@@ -2315,15 +2315,15 @@
       <c r="H55" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I55" s="28"/>
+      <c r="I55" s="31"/>
     </row>
     <row r="56" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B56" s="23"/>
-      <c r="C56" s="24"/>
+      <c r="B56" s="26"/>
+      <c r="C56" s="27"/>
       <c r="D56" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E56" s="27"/>
+      <c r="E56" s="30"/>
       <c r="F56" s="8">
         <v>0.80100000000000005</v>
       </c>
@@ -2333,41 +2333,26 @@
       <c r="H56" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I56" s="28"/>
+      <c r="I56" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="E45:E47"/>
-    <mergeCell ref="I45:I47"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="I33:I35"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="I51:I53"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="I8:I11"/>
-    <mergeCell ref="I27:I29"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="I30:I32"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="I42:I44"/>
-    <mergeCell ref="I36:I38"/>
-    <mergeCell ref="I39:I41"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="E54:E56"/>
+    <mergeCell ref="I54:I56"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="E48:E50"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="E42:E44"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="B21:B23"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="B12:B14"/>
@@ -2384,22 +2369,37 @@
     <mergeCell ref="C42:C44"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="C54:C56"/>
-    <mergeCell ref="E54:E56"/>
-    <mergeCell ref="I54:I56"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="E48:E50"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="E42:E44"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="I51:I53"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="I8:I11"/>
+    <mergeCell ref="I27:I29"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I30:I32"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="I42:I44"/>
+    <mergeCell ref="I36:I38"/>
+    <mergeCell ref="I39:I41"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="E45:E47"/>
+    <mergeCell ref="I45:I47"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="I33:I35"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="E39:E41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2409,8 +2409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB266944-C992-CA4E-B72E-F8C46C08F0CD}">
   <dimension ref="B2:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2426,7 +2426,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="20" x14ac:dyDescent="0.2">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="23" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2457,122 +2457,122 @@
       </c>
     </row>
     <row r="4" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="24" t="s">
         <v>57</v>
       </c>
       <c r="E4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="39">
-        <v>0.7036</v>
+      <c r="F4" s="25">
+        <v>0.72160000000000002</v>
       </c>
       <c r="G4" s="8">
-        <v>0.76070000000000004</v>
+        <v>0.77980000000000005</v>
       </c>
       <c r="H4" s="8">
-        <v>0.82140000000000002</v>
+        <v>0.83730000000000004</v>
       </c>
       <c r="I4" s="8">
-        <v>0.78339999999999999</v>
+        <v>0.80269999999999997</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="29"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="38" t="s">
+      <c r="B5" s="33"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="24" t="s">
         <v>58</v>
       </c>
       <c r="E5" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F5" s="8">
-        <v>0.73219999999999996</v>
-      </c>
-      <c r="G5" s="39">
-        <v>0.74880000000000002</v>
+        <v>0.74539999999999995</v>
+      </c>
+      <c r="G5" s="25">
+        <v>0.77</v>
       </c>
       <c r="H5" s="8">
-        <v>0.81810000000000005</v>
+        <v>0.83620000000000005</v>
       </c>
       <c r="I5" s="8">
-        <v>0.78200000000000003</v>
+        <v>0.80330000000000001</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="73" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="29"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="38" t="s">
+      <c r="B6" s="33"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="24" t="s">
         <v>59</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F6" s="8">
-        <v>0.73260000000000003</v>
+        <v>0.745</v>
       </c>
       <c r="G6" s="8">
-        <v>0.76</v>
-      </c>
-      <c r="H6" s="39">
-        <v>0.80600000000000005</v>
+        <v>0.77759999999999996</v>
+      </c>
+      <c r="H6" s="25">
+        <v>0.81579999999999997</v>
       </c>
       <c r="I6" s="8">
-        <v>0.77649999999999997</v>
+        <v>0.79579999999999995</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="29"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="38" t="s">
+      <c r="B7" s="33"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="24" t="s">
         <v>60</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="8">
-        <v>0.72550000000000003</v>
+        <v>0.74299999999999999</v>
       </c>
       <c r="G7" s="8">
-        <v>0.75900000000000001</v>
+        <v>0.77849999999999997</v>
       </c>
       <c r="H7" s="8">
-        <v>0.81520000000000004</v>
-      </c>
-      <c r="I7" s="39">
-        <v>0.77580000000000005</v>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="I7" s="25">
+        <v>0.79690000000000005</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="74" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="29"/>
-      <c r="C8" s="24"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="15" t="s">
         <v>61</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="39">
-        <v>0.67120000000000002</v>
-      </c>
-      <c r="G8" s="39">
-        <v>0.73419999999999996</v>
+      <c r="F8" s="25">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="G8" s="25">
+        <v>0.75229999999999997</v>
       </c>
       <c r="H8" s="8">
-        <v>0.82820000000000005</v>
+        <v>0.84370000000000001</v>
       </c>
       <c r="I8" s="8">
-        <v>0.78790000000000004</v>
+        <v>0.80740000000000001</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="21" x14ac:dyDescent="0.2">
-      <c r="B9" s="29"/>
-      <c r="C9" s="24"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="15" t="s">
         <v>62</v>
       </c>
@@ -2580,21 +2580,21 @@
         <v>25</v>
       </c>
       <c r="F9" s="8">
-        <v>0.7319</v>
+        <v>0.74709999999999999</v>
       </c>
       <c r="G9" s="8">
-        <v>0.7601</v>
-      </c>
-      <c r="H9" s="39">
-        <v>0.79600000000000004</v>
-      </c>
-      <c r="I9" s="39">
-        <v>0.76590000000000003</v>
+        <v>0.77959999999999996</v>
+      </c>
+      <c r="H9" s="25">
+        <v>0.80289999999999995</v>
+      </c>
+      <c r="I9" s="25">
+        <v>0.78749999999999998</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="21" x14ac:dyDescent="0.2">
-      <c r="B10" s="29"/>
-      <c r="C10" s="24"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="15" t="s">
         <v>63</v>
       </c>
@@ -2602,82 +2602,82 @@
         <v>25</v>
       </c>
       <c r="F10" s="8">
-        <v>0.75309999999999999</v>
-      </c>
-      <c r="G10" s="39">
-        <v>0.73009999999999997</v>
-      </c>
-      <c r="H10" s="39">
-        <v>0.75270000000000004</v>
-      </c>
-      <c r="I10" s="39">
-        <v>0.7399</v>
+        <v>0.7621</v>
+      </c>
+      <c r="G10" s="25">
+        <v>0.75590000000000002</v>
+      </c>
+      <c r="H10" s="25">
+        <v>0.77569999999999995</v>
+      </c>
+      <c r="I10" s="25">
+        <v>0.77090000000000003</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="21" x14ac:dyDescent="0.2">
-      <c r="B11" s="29"/>
-      <c r="C11" s="24"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="15" t="s">
         <v>65</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="39">
-        <v>0.6784</v>
+      <c r="F11" s="25">
+        <v>0.72219999999999995</v>
       </c>
       <c r="G11" s="8">
-        <v>0.7339</v>
-      </c>
-      <c r="H11" s="39">
-        <v>0.81659999999999999</v>
-      </c>
-      <c r="I11" s="39">
-        <v>0.78920000000000001</v>
+        <v>0.78249999999999997</v>
+      </c>
+      <c r="H11" s="25">
+        <v>0.80879999999999996</v>
+      </c>
+      <c r="I11" s="25">
+        <v>0.78769999999999996</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="21" x14ac:dyDescent="0.2">
-      <c r="B12" s="29"/>
-      <c r="C12" s="24"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="15" t="s">
         <v>64</v>
       </c>
       <c r="E12" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="39">
-        <v>0.65759999999999996</v>
-      </c>
-      <c r="G12" s="39">
-        <v>0.72699999999999998</v>
+      <c r="F12" s="25">
+        <v>0.68089999999999995</v>
+      </c>
+      <c r="G12" s="25">
+        <v>0.75319999999999998</v>
       </c>
       <c r="H12" s="8">
-        <v>0.82820000000000005</v>
-      </c>
-      <c r="I12" s="39">
-        <v>0.77759999999999996</v>
+        <v>0.84470000000000001</v>
+      </c>
+      <c r="I12" s="25">
+        <v>0.79790000000000005</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="21" x14ac:dyDescent="0.2">
-      <c r="B13" s="29"/>
-      <c r="C13" s="24"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="15" t="s">
         <v>66</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="39">
-        <v>0.68079999999999996</v>
-      </c>
-      <c r="G13" s="39">
-        <v>0.73560000000000003</v>
-      </c>
-      <c r="H13" s="39">
-        <v>0.81589999999999996</v>
+      <c r="F13" s="25">
+        <v>0.69720000000000004</v>
+      </c>
+      <c r="G13" s="25">
+        <v>0.75580000000000003</v>
+      </c>
+      <c r="H13" s="25">
+        <v>0.83220000000000005</v>
       </c>
       <c r="I13" s="8">
-        <v>0.78810000000000002</v>
+        <v>0.80740000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Experimented with more hyperparameters
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yimenggu/Desktop/twitter-comms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FAE84A-CC11-9F4F-96C5-6FDDB5D01A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E533D7-9509-2745-875B-38F31ACBE4E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29080" yWindow="880" windowWidth="28800" windowHeight="15920" activeTab="2" xr2:uid="{83E1EE90-11A9-2944-8CCC-8774B4B18D7B}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="28800" windowHeight="15920" activeTab="2" xr2:uid="{83E1EE90-11A9-2944-8CCC-8774B4B18D7B}"/>
   </bookViews>
   <sheets>
     <sheet name="MLLMs" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="127">
   <si>
     <t>No.</t>
   </si>
@@ -351,6 +351,81 @@
   </si>
   <si>
     <t>0.8074 / 0.793</t>
+  </si>
+  <si>
+    <t>ctr weight increased to 50x</t>
+  </si>
+  <si>
+    <t>0.679 / 0.709</t>
+  </si>
+  <si>
+    <t>0.7523 / 0.754</t>
+  </si>
+  <si>
+    <t>0.8437 / 0.828</t>
+  </si>
+  <si>
+    <t>0.8074 / 0.799</t>
+  </si>
+  <si>
+    <t>0.8029 / 0.79</t>
+  </si>
+  <si>
+    <t>0.7875 / 0.769</t>
+  </si>
+  <si>
+    <t>0.7471 / 0.738</t>
+  </si>
+  <si>
+    <t>0.7796 / 0.763</t>
+  </si>
+  <si>
+    <t>ctr weight increased to 75x</t>
+  </si>
+  <si>
+    <t>0.8029 / 0.794</t>
+  </si>
+  <si>
+    <t>0.7875 / 0.771</t>
+  </si>
+  <si>
+    <t>0.7471 / 0.737</t>
+  </si>
+  <si>
+    <t>0.7796 / 0.76</t>
+  </si>
+  <si>
+    <t>0.679 / 0.711</t>
+  </si>
+  <si>
+    <t>0.8437 / 0.825</t>
+  </si>
+  <si>
+    <t>0.8074 / 0.794</t>
+  </si>
+  <si>
+    <t>0.679 / 0.715</t>
+  </si>
+  <si>
+    <t>0.7523 / 0.759</t>
+  </si>
+  <si>
+    <t>0.8074 / 0.798</t>
+  </si>
+  <si>
+    <t>ctr weight increased to 75x, learning rate increased from 2e-4 to 1e-4, to match blip-2+linear</t>
+  </si>
+  <si>
+    <t>0.8029 / 0.8</t>
+  </si>
+  <si>
+    <t>0.7875 / 0.773</t>
+  </si>
+  <si>
+    <t>0.7471 / 0.74</t>
+  </si>
+  <si>
+    <t>0.7796 / 0.764</t>
   </si>
 </sst>
 </file>
@@ -515,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -615,6 +690,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -636,11 +714,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1175,10 +1253,10 @@
       <c r="M3" s="13"/>
     </row>
     <row r="4" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="42" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="15" t="s">
@@ -1196,15 +1274,15 @@
       <c r="H4" s="8">
         <v>0.71699999999999997</v>
       </c>
-      <c r="I4" s="44"/>
+      <c r="I4" s="37"/>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
     </row>
     <row r="5" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B5" s="39"/>
-      <c r="C5" s="42"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="17" t="s">
         <v>30</v>
       </c>
@@ -1220,15 +1298,15 @@
       <c r="H5" s="8">
         <v>0.80800000000000005</v>
       </c>
-      <c r="I5" s="44"/>
+      <c r="I5" s="37"/>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
     </row>
     <row r="6" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B6" s="39"/>
-      <c r="C6" s="42"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="15" t="s">
         <v>31</v>
       </c>
@@ -1244,15 +1322,15 @@
       <c r="H6" s="8">
         <v>0.81100000000000005</v>
       </c>
-      <c r="I6" s="44"/>
+      <c r="I6" s="37"/>
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
     </row>
     <row r="7" spans="2:13" ht="21" x14ac:dyDescent="0.2">
-      <c r="B7" s="40"/>
-      <c r="C7" s="43"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="15" t="s">
         <v>23</v>
       </c>
@@ -1268,14 +1346,14 @@
       <c r="H7" s="8">
         <v>0.81100000000000005</v>
       </c>
-      <c r="I7" s="44"/>
+      <c r="I7" s="37"/>
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
       <c r="M7" s="13"/>
     </row>
     <row r="8" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="38" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="32" t="s">
@@ -1296,14 +1374,14 @@
       <c r="H8" s="8">
         <v>0.63700000000000001</v>
       </c>
-      <c r="I8" s="44"/>
+      <c r="I8" s="37"/>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
     </row>
     <row r="9" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B9" s="37"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="32"/>
       <c r="D9" s="17" t="s">
         <v>30</v>
@@ -1320,14 +1398,14 @@
       <c r="H9" s="8">
         <v>0.69299999999999995</v>
       </c>
-      <c r="I9" s="44"/>
+      <c r="I9" s="37"/>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
     </row>
     <row r="10" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B10" s="37"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="32"/>
       <c r="D10" s="15" t="s">
         <v>31</v>
@@ -1344,14 +1422,14 @@
       <c r="H10" s="8">
         <v>0.69799999999999995</v>
       </c>
-      <c r="I10" s="44"/>
+      <c r="I10" s="37"/>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
     </row>
     <row r="11" spans="2:13" ht="20" x14ac:dyDescent="0.2">
-      <c r="B11" s="37"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="32"/>
       <c r="D11" s="19" t="s">
         <v>23</v>
@@ -1368,14 +1446,14 @@
       <c r="H11" s="8">
         <v>0.69699999999999995</v>
       </c>
-      <c r="I11" s="44"/>
+      <c r="I11" s="37"/>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
     </row>
     <row r="12" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="38" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="32" t="s">
@@ -1396,14 +1474,14 @@
       <c r="H12" s="8">
         <v>0.72099999999999997</v>
       </c>
-      <c r="I12" s="44"/>
+      <c r="I12" s="37"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
     </row>
     <row r="13" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B13" s="37"/>
+      <c r="B13" s="38"/>
       <c r="C13" s="32"/>
       <c r="D13" s="17" t="s">
         <v>30</v>
@@ -1420,14 +1498,14 @@
       <c r="H13" s="8">
         <v>0.76800000000000002</v>
       </c>
-      <c r="I13" s="44"/>
+      <c r="I13" s="37"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
     </row>
     <row r="14" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B14" s="37"/>
+      <c r="B14" s="38"/>
       <c r="C14" s="32"/>
       <c r="D14" s="15" t="s">
         <v>31</v>
@@ -1444,14 +1522,14 @@
       <c r="H14" s="8">
         <v>0.77</v>
       </c>
-      <c r="I14" s="44"/>
+      <c r="I14" s="37"/>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
     </row>
     <row r="15" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="38" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="32" t="s">
@@ -1472,14 +1550,14 @@
       <c r="H15" s="8">
         <v>0.78400000000000003</v>
       </c>
-      <c r="I15" s="44"/>
+      <c r="I15" s="37"/>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
     </row>
     <row r="16" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B16" s="37"/>
+      <c r="B16" s="38"/>
       <c r="C16" s="32"/>
       <c r="D16" s="17" t="s">
         <v>30</v>
@@ -1494,14 +1572,14 @@
       <c r="H16" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="44"/>
+      <c r="I16" s="37"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
     </row>
     <row r="17" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B17" s="37"/>
+      <c r="B17" s="38"/>
       <c r="C17" s="32"/>
       <c r="D17" s="15" t="s">
         <v>31</v>
@@ -1516,14 +1594,14 @@
       <c r="H17" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="44"/>
+      <c r="I17" s="37"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
     </row>
     <row r="18" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="38" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="32" t="s">
@@ -1544,14 +1622,14 @@
       <c r="H18" s="8">
         <v>0.78500000000000003</v>
       </c>
-      <c r="I18" s="44"/>
+      <c r="I18" s="37"/>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
     </row>
     <row r="19" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B19" s="37"/>
+      <c r="B19" s="38"/>
       <c r="C19" s="32"/>
       <c r="D19" s="17" t="s">
         <v>30</v>
@@ -1566,14 +1644,14 @@
       <c r="H19" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="44"/>
+      <c r="I19" s="37"/>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
     </row>
     <row r="20" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B20" s="37"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="32"/>
       <c r="D20" s="15" t="s">
         <v>31</v>
@@ -1588,7 +1666,7 @@
       <c r="H20" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="44"/>
+      <c r="I20" s="37"/>
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
@@ -2331,7 +2409,7 @@
       <c r="M50" s="13"/>
     </row>
     <row r="51" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B51" s="37" t="s">
+      <c r="B51" s="38" t="s">
         <v>22</v>
       </c>
       <c r="C51" s="32" t="s">
@@ -2352,14 +2430,14 @@
       <c r="H51" s="8">
         <v>0.75600000000000001</v>
       </c>
-      <c r="I51" s="44"/>
+      <c r="I51" s="37"/>
       <c r="J51" s="13"/>
       <c r="K51" s="13"/>
       <c r="L51" s="13"/>
       <c r="M51" s="13"/>
     </row>
     <row r="52" spans="2:13" ht="42" x14ac:dyDescent="0.2">
-      <c r="B52" s="37"/>
+      <c r="B52" s="38"/>
       <c r="C52" s="32"/>
       <c r="D52" s="17" t="s">
         <v>30</v>
@@ -2376,14 +2454,14 @@
       <c r="H52" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I52" s="44"/>
+      <c r="I52" s="37"/>
       <c r="J52" s="13"/>
       <c r="K52" s="13"/>
       <c r="L52" s="13"/>
       <c r="M52" s="13"/>
     </row>
     <row r="53" spans="2:13" ht="63" x14ac:dyDescent="0.2">
-      <c r="B53" s="37"/>
+      <c r="B53" s="38"/>
       <c r="C53" s="32"/>
       <c r="D53" s="15" t="s">
         <v>31</v>
@@ -2400,7 +2478,7 @@
       <c r="H53" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I53" s="44"/>
+      <c r="I53" s="37"/>
     </row>
     <row r="54" spans="2:13" ht="42" x14ac:dyDescent="0.2">
       <c r="B54" s="31" t="s">
@@ -2466,37 +2544,22 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="E45:E47"/>
-    <mergeCell ref="I45:I47"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="I33:I35"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="I51:I53"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="I8:I11"/>
-    <mergeCell ref="I27:I29"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="I30:I32"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="I42:I44"/>
-    <mergeCell ref="I36:I38"/>
-    <mergeCell ref="I39:I41"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="E54:E56"/>
+    <mergeCell ref="I54:I56"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="E48:E50"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="E42:E44"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="B21:B23"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="B12:B14"/>
@@ -2513,22 +2576,37 @@
     <mergeCell ref="C42:C44"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="C54:C56"/>
-    <mergeCell ref="E54:E56"/>
-    <mergeCell ref="I54:I56"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="E48:E50"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="E42:E44"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="I51:I53"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="I8:I11"/>
+    <mergeCell ref="I27:I29"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I30:I32"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="I42:I44"/>
+    <mergeCell ref="I36:I38"/>
+    <mergeCell ref="I39:I41"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="E45:E47"/>
+    <mergeCell ref="I45:I47"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="I33:I35"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="E39:E41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2536,10 +2614,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB266944-C992-CA4E-B72E-F8C46C08F0CD}">
-  <dimension ref="B2:J24"/>
+  <dimension ref="B2:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="B20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3064,11 +3142,146 @@
         <v>78</v>
       </c>
     </row>
+    <row r="25" spans="4:10" ht="42" x14ac:dyDescent="0.2">
+      <c r="D25" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="G25" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="H25" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="I25" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="J25" s="45" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="4:10" ht="21" x14ac:dyDescent="0.2">
+      <c r="D26" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="G26" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="H26" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="I26" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="J26" s="45"/>
+    </row>
+    <row r="27" spans="4:10" ht="42" x14ac:dyDescent="0.2">
+      <c r="D27" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="G27" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="H27" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="I27" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="J27" s="45" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="4:10" ht="21" x14ac:dyDescent="0.2">
+      <c r="D28" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="G28" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="H28" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="I28" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="J28" s="45"/>
+    </row>
+    <row r="29" spans="4:10" ht="42" x14ac:dyDescent="0.2">
+      <c r="D29" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="G29" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="H29" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="I29" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="J29" s="46" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="4:10" ht="21" x14ac:dyDescent="0.2">
+      <c r="D30" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="H30" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="I30" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="J30" s="46"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="J29:J30"/>
     <mergeCell ref="J15:J16"/>
     <mergeCell ref="C4:C16"/>
     <mergeCell ref="B4:B16"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="J27:J28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>